<commit_message>
useful excel 2013 for std error of means and confidence interval
</commit_message>
<xml_diff>
--- a/StdErr_and_ConfidenceInterval.xlsx
+++ b/StdErr_and_ConfidenceInterval.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Docz\Corsi\6sigma - Black Belt\versione01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\_internal\six-sigma-git\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -211,8 +211,8 @@
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="112980" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="CasellaDiTesto 1"/>
@@ -248,6 +248,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -271,7 +272,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -287,7 +288,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="CasellaDiTesto 1"/>
@@ -363,8 +364,8 @@
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="117853" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="CasellaDiTesto 2"/>
@@ -400,6 +401,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -434,7 +436,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="CasellaDiTesto 2"/>
@@ -493,8 +495,8 @@
       <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="179793" cy="193771"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="CasellaDiTesto 3"/>
@@ -530,6 +532,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -563,7 +566,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -590,7 +593,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="CasellaDiTesto 3"/>
@@ -680,8 +683,8 @@
       <xdr:rowOff>155438</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="846514" cy="275525"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="CasellaDiTesto 4"/>
@@ -717,6 +720,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -757,7 +761,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -770,7 +774,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -811,7 +815,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="CasellaDiTesto 4"/>
@@ -901,8 +905,8 @@
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1666995" cy="380361"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="CasellaDiTesto 5"/>
@@ -938,6 +942,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -975,7 +980,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -988,7 +993,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -1002,7 +1007,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -1018,7 +1023,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -1033,7 +1038,7 @@
                                       <a:schemeClr val="tx1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -1046,7 +1051,7 @@
                                       <a:schemeClr val="tx1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -1058,7 +1063,7 @@
                                       <a:schemeClr val="tx1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -1072,7 +1077,7 @@
                                       <a:schemeClr val="tx1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -1092,7 +1097,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="CasellaDiTesto 5"/>
@@ -1168,8 +1173,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1768475</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>60325</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
@@ -1183,7 +1188,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="1768475" y="4057650"/>
+              <a:off x="1901825" y="4057650"/>
               <a:ext cx="2125069" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1211,6 +1216,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1312,7 +1318,7 @@
                                         <a:schemeClr val="tx1"/>
                                       </a:solidFill>
                                       <a:effectLst/>
-                                      <a:latin typeface="+mn-lt"/>
+                                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                       <a:ea typeface="+mn-ea"/>
                                       <a:cs typeface="+mn-cs"/>
                                     </a:rPr>
@@ -1325,7 +1331,7 @@
                                         <a:schemeClr val="tx1"/>
                                       </a:solidFill>
                                       <a:effectLst/>
-                                      <a:latin typeface="+mn-lt"/>
+                                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                       <a:ea typeface="+mn-ea"/>
                                       <a:cs typeface="+mn-cs"/>
                                     </a:rPr>
@@ -1351,7 +1357,7 @@
                                     <a:schemeClr val="tx1"/>
                                   </a:solidFill>
                                   <a:effectLst/>
-                                  <a:latin typeface="+mn-lt"/>
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                   <a:ea typeface="+mn-ea"/>
                                   <a:cs typeface="+mn-cs"/>
                                 </a:rPr>
@@ -1363,7 +1369,7 @@
                                     <a:schemeClr val="tx1"/>
                                   </a:solidFill>
                                   <a:effectLst/>
-                                  <a:latin typeface="+mn-lt"/>
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                   <a:ea typeface="+mn-ea"/>
                                   <a:cs typeface="+mn-cs"/>
                                 </a:rPr>
@@ -1375,7 +1381,7 @@
                                     <a:schemeClr val="tx1"/>
                                   </a:solidFill>
                                   <a:effectLst/>
-                                  <a:latin typeface="+mn-lt"/>
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                   <a:ea typeface="+mn-ea"/>
                                   <a:cs typeface="+mn-cs"/>
                                 </a:rPr>
@@ -1402,7 +1408,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="1768475" y="4057650"/>
+              <a:off x="1901825" y="4057650"/>
               <a:ext cx="2125069" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1430,6 +1436,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="it-IT" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -1455,47 +1462,11 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>𝜇 ̂</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="it-IT" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>+</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="it-IT" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>𝑘∗𝑆𝐸𝑀</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="it-IT" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>)┤[</a:t>
+                <a:t>𝜇 ̂+𝑘∗𝑆𝐸𝑀)┤[</a:t>
               </a:r>
               <a:endParaRPr lang="it-IT" sz="1100"/>
             </a:p>
@@ -1773,13 +1744,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.453125" customWidth="1"/>
+    <col min="1" max="1" width="26.36328125" customWidth="1"/>
     <col min="3" max="3" width="23.90625" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
   </cols>

</xml_diff>